<commit_message>
Modif. DB-Campo observacion (tabla historico). Modif. DB-Campo id_persona (tabla historico). Modif. ABM historico, manejo de comentarios entre paso de estados. Nuevo modulo. Detalle historico registros. Generacion script para manejo de DB.
</commit_message>
<xml_diff>
--- a/archivos/03 - Querys Insert workflow/Datos workflow.xlsx
+++ b/archivos/03 - Querys Insert workflow/Datos workflow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="4" windowWidth="15090" windowHeight="6510"/>
+    <workbookView activeTab="3" windowWidth="15090" windowHeight="6510"/>
   </bookViews>
   <sheets>
     <sheet name="TipoEvento" sheetId="1" r:id="rId1"/>
@@ -117,22 +117,22 @@
     <t>INSERT INTO sgr.estado(id_estado, nombre, inicio, fin) values (7,'CANCELADO',FALSE,TRUE);</t>
   </si>
   <si>
-    <t>INSERT INTO sgr.workflow(id_workflow, nombre,id_evento) values (</t>
-  </si>
-  <si>
-    <t>INSERT INTO sgr.workflow(id_workflow, nombre,id_evento) values (1,'RECEPCION FC TELECOM',2);</t>
-  </si>
-  <si>
-    <t>INSERT INTO sgr.workflow(id_workflow, nombre,id_evento) values (2,'RECEPCION FC CVI',2);</t>
-  </si>
-  <si>
-    <t>INSERT INTO sgr.workflow(id_workflow, nombre,id_evento) values (3,'RECEPCION FC BBT',2);</t>
-  </si>
-  <si>
-    <t>INSERT INTO sgr.workflow(id_workflow, nombre,id_evento) values (4,'RECEPCION DE CV',1);</t>
-  </si>
-  <si>
-    <t>INSERT INTO sgr.workflow(id_workflow, nombre,id_evento) values (5,'LLAMADA DE PARQUES NACIONALES',5);</t>
+    <t>INSERT INTO sgr.workflow(id_workflow, nombre,id_evento,id_dpto,notifica) values (</t>
+  </si>
+  <si>
+    <t>INSERT INTO sgr.workflow(id_workflow, nombre,id_evento,id_dpto,notifica) values (1,'RECEPCION FC TELECOM',2,6);</t>
+  </si>
+  <si>
+    <t>INSERT INTO sgr.workflow(id_workflow, nombre,id_evento,id_dpto,notifica) values (2,'RECEPCION FC CVI',2,6);</t>
+  </si>
+  <si>
+    <t>INSERT INTO sgr.workflow(id_workflow, nombre,id_evento,id_dpto,notifica) values (3,'RECEPCION FC BBT',2,6);</t>
+  </si>
+  <si>
+    <t>INSERT INTO sgr.workflow(id_workflow, nombre,id_evento,id_dpto,notifica) values (4,'RECEPCION DE CV',1,13);</t>
+  </si>
+  <si>
+    <t>INSERT INTO sgr.workflow(id_workflow, nombre,id_evento,id_dpto,notifica) values (5,'LLAMADA DE PARQUES NACIONALES',5,8);</t>
   </si>
   <si>
     <t>INSERT INTO sgr.flujo(id_workflow,id_estadoorigen,id_estadodestino,orden) values (</t>
@@ -1090,22 +1090,22 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I6"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <selection activeCell="K2" sqref="K2:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" style="0" width="4.428305288461539" customWidth="1"/>
     <col min="2" max="2" style="0" width="17.42752403846154" customWidth="1"/>
-    <col min="3" max="5" style="0" width="9.142307692307693"/>
-    <col min="6" max="6" style="0" width="42.283173076923084" customWidth="1"/>
-    <col min="7" max="16384" style="0" width="9.142307692307693"/>
+    <col min="3" max="7" style="0" width="9.142307692307693"/>
+    <col min="8" max="8" style="0" width="42.283173076923084" customWidth="1"/>
+    <col min="9" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1117,8 +1117,18 @@
           <t>id_evt</t>
         </is>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>id_dpto</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>notifica</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1130,22 +1140,28 @@
       <c r="C2">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" t="str">
-        <f>A2&amp;","&amp;"'"&amp;B2&amp;"'"&amp;","&amp;C2&amp;")"</f>
-        <v>1,'RECEPCION FC TELECOM',2)</v>
-      </c>
-      <c r="H2" t="s">
-        <f>E2&amp;F2&amp;";"</f>
+      <c r="H2" t="str">
+        <f>A2&amp;","&amp;"'"&amp;B2&amp;"'"&amp;","&amp;C2&amp;","&amp;D2&amp;")"</f>
+        <v>1,'RECEPCION FC TELECOM',2,6)</v>
+      </c>
+      <c r="J2" t="s">
+        <f>G2&amp;H2&amp;";"</f>
         <v>29</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1157,22 +1173,28 @@
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" t="str">
-        <f>A3&amp;","&amp;"'"&amp;B3&amp;"'"&amp;","&amp;C3&amp;")"</f>
-        <v>2,'RECEPCION FC CVI',2)</v>
-      </c>
-      <c r="H3" t="s">
-        <f>E3&amp;F3&amp;";"</f>
+      <c r="H3" t="str">
+        <f>A3&amp;","&amp;"'"&amp;B3&amp;"'"&amp;","&amp;C3&amp;","&amp;D3&amp;")"</f>
+        <v>2,'RECEPCION FC CVI',2,6)</v>
+      </c>
+      <c r="J3" t="s">
+        <f>G3&amp;H3&amp;";"</f>
         <v>30</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1184,22 +1206,28 @@
       <c r="C4">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
         <v>28</v>
       </c>
-      <c r="F4" t="str">
-        <f>A4&amp;","&amp;"'"&amp;B4&amp;"'"&amp;","&amp;C4&amp;")"</f>
-        <v>3,'RECEPCION FC BBT',2)</v>
-      </c>
-      <c r="H4" t="s">
-        <f>E4&amp;F4&amp;";"</f>
+      <c r="H4" t="str">
+        <f>A4&amp;","&amp;"'"&amp;B4&amp;"'"&amp;","&amp;C4&amp;","&amp;D4&amp;")"</f>
+        <v>3,'RECEPCION FC BBT',2,6)</v>
+      </c>
+      <c r="J4" t="s">
+        <f>G4&amp;H4&amp;";"</f>
         <v>31</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1211,22 +1239,28 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D5">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
         <v>28</v>
       </c>
-      <c r="F5" t="str">
-        <f>A5&amp;","&amp;"'"&amp;B5&amp;"'"&amp;","&amp;C5&amp;")"</f>
-        <v>4,'RECEPCION DE CV',1)</v>
-      </c>
-      <c r="H5" t="s">
-        <f>E5&amp;F5&amp;";"</f>
+      <c r="H5" t="str">
+        <f>A5&amp;","&amp;"'"&amp;B5&amp;"'"&amp;","&amp;C5&amp;","&amp;D5&amp;")"</f>
+        <v>4,'RECEPCION DE CV',1,13)</v>
+      </c>
+      <c r="J5" t="s">
+        <f>G5&amp;H5&amp;";"</f>
         <v>32</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1238,19 +1272,44 @@
       <c r="C6">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
         <v>28</v>
       </c>
-      <c r="F6" t="str">
-        <f>A6&amp;","&amp;"'"&amp;B6&amp;"'"&amp;","&amp;C6&amp;")"</f>
-        <v>5,'LLAMADA DE PARQUES NACIONALES',5)</v>
-      </c>
-      <c r="H6" t="s">
-        <f>E6&amp;F6&amp;";"</f>
+      <c r="H6" t="str">
+        <f>A6&amp;","&amp;"'"&amp;B6&amp;"'"&amp;","&amp;C6&amp;","&amp;D6&amp;")"</f>
+        <v>5,'LLAMADA DE PARQUES NACIONALES',5,8)</v>
+      </c>
+      <c r="J6" t="s">
+        <f>G6&amp;H6&amp;";"</f>
         <v>33</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>LAPOS</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1272,8 +1331,8 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0" tabSelected="1">
-      <selection activeCell="J44" sqref="J44:J55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>